<commit_message>
yay! documented parts list
</commit_message>
<xml_diff>
--- a/partslist.xlsx
+++ b/partslist.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4540"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8530"/>
   </bookViews>
   <sheets>
     <sheet name="output" sheetId="1" r:id="rId1"/>
@@ -36,169 +36,169 @@
     <t>id14</t>
   </si>
   <si>
-    <t>GAAGACTCTGGCGGTTCATGCAGTTGTTCGGGCACCATCAGCCCCTACGGCCTGCGCACTTGTCGCGCGACTAAGACGAAACCATCGCATCCGACCACGAAAGAAACACATCCGCAGACGCTTCCGACGTCTTCTGTCTTC</t>
+    <t>GAAGACTCTGGCGGTTCATGCAGTTGTTCGGGCACCATCAGCCCCTACGGCCTGCGCACTTGTCGCGCGACTAAGACGAAACCATCGCATCCGACCACGAAAGAAACACATCCGCAGACGCTTCCGACGTCGTCTGTCTTC</t>
   </si>
   <si>
     <t>id15</t>
   </si>
   <si>
-    <t>GAAGACTCTGGCTATGTCAGTTGCTTGTTTCGTGGTGCCCGTTGCCGTGTATATTCGGGTCGTTCATGTTGCTTTGGCTACTACTGCCGTCGTGACTTTCCTGGGTCGATCTTCGGGACTTGTTCCCGTCGCAACTTTTCTTCTGTCTTC</t>
+    <t>GAAGACTCTGGCTATGTCAGTTGCTTGTTTCGTGGTGCCCGTTGCCGTGTATATTCGGGTCGTTCATGTTGCTTTGGCTACTACTGCCGTCGTGACTTTCCTGGGTCGATCTTCGGGACTTGTTCCCGTCGCAACTTTTCGTCTGTCTTC</t>
   </si>
   <si>
     <t>id16</t>
   </si>
   <si>
-    <t>GAAGACTCTGGCGCACGTTCCTACGGCAATGGGGTATATTGCAATAACAAGAAGTGTTGGGTGAATCGCGGGGAGGCGACTCAGAGCATCATTGGAGGTATGATCTCAGGGTGGGCGAGCGGGTTAGCGGGAATGTCTTCTGTCTTC</t>
+    <t>GAAGACTCTGGCGCACGTTCCTACGGCAATGGGGTATATTGCAATAACAAGAAGTGTTGGGTGAATCGCGGGGAGGCGACTCAGAGCATCATTGGAGGTATGATCTCAGGGTGGGCGAGCGGGTTAGCGGGAATGTCGTCTGTCTTC</t>
   </si>
   <si>
     <t>id17</t>
   </si>
   <si>
-    <t>GAAGACTCTGGCCAAGTTTACAAGGGCGGATACACACGTCCAATTCCTCGTCCCCCCCCATTCGTCCGTCCTCTTCCTGGTGGCCCGATTGGCCCGTACAATGGATGTCCGGTGTCGTGCCGTGGAATTTCGTTCAGCCAAGCCCGTAGCTGTTGCTCCCGTCTGGGACGTTGTTGCCATGTTGGAAAGGGGTATTCTTCTTCTGTCTTC</t>
+    <t>GAAGACTCTGGCCAAGTTTACAAGGGCGGATACACACGTCCAATTCCTCGTCCCCCCCCATTCGTCCGTCCTCTTCCTGGTGGCCCGATTGGCCCGTACAATGGATGTCCGGTGTCGTGCCGTGGAATTTCGTTCAGCCAAGCCCGTAGCTGTTGCTCCCGTCTGGGACGTTGTTGCCATGTTGGAAAGGGGTATTCTTCGTCTGTCTTC</t>
   </si>
   <si>
     <t>id18</t>
   </si>
   <si>
-    <t>GAAGACTCTGGCAAACCAGCTTGGTGCTGGTACACACTGGCAATGTGTGGGGCCGGGTACGATTCGGGCACTTGTGATTATATGTATAGCCACTGCTTCGGAGTAAAGCACTCATCGGGGGGAGGTGGGTCTTACCACTGCTCTTCTGTCTTC</t>
+    <t>GAAGACTCTGGCAAACCAGCTTGGTGCTGGTACACACTGGCAATGTGTGGGGCCGGGTACGATTCGGGCACTTGTGATTATATGTATAGCCACTGCTTCGGAGTAAAGCACTCATCGGGGGGAGGTGGGTCTTACCACTGCTCGTCTGTCTTC</t>
   </si>
   <si>
     <t>id19</t>
   </si>
   <si>
-    <t>GAAGACTCTGGCGCCACCTGCGACTTGCTGTCGATTAGCACCCCGTGGGGCAGTGTCAACCACGCTGCGTGTGCTGCCCACTGCTTGGCCCTTAATCGCGGTTTTCGTGGCGGTTATTGCTCCTCAAAGGCGGTGTGTACTTGTCGCAAGTCTTCTGTCTTC</t>
+    <t>GAAGACTCTGGCGCCACCTGCGACTTGCTGTCGATTAGCACCCCGTGGGGCAGTGTCAACCACGCTGCGTGTGCTGCCCACTGCTTGGCCCTTAATCGCGGTTTTCGTGGCGGTTATTGCTCCTCAAAGGCGGTGTGTACTTGTCGCAAGTCGTCTGTCTTC</t>
   </si>
   <si>
     <t>id20</t>
   </si>
   <si>
-    <t>GAAGACTCTGGCCACCGTCACCAAGGGCCAATTTTCGACACTCGTCCATCACCCTTTAACCCAAATCAGCCCCGCCCGGGGCCCATTTATTCTTCTGTCTTC</t>
+    <t>GAAGACTCTGGCCACCGTCACCAAGGGCCAATTTTCGACACTCGTCCATCACCCTTTAACCCAAATCAGCCCCGCCCGGGGCCCATTTATTCGTCTGTCTTC</t>
   </si>
   <si>
     <t>id21</t>
   </si>
   <si>
-    <t>GAAGACTCTGGCGGTATCTGGAGCTCAATCAAGAATTTAGCGTCAAAAGCCTGGAATAGCGACATCGGCCAGTCACTGCGTAACAAAGCGGCGGGCGCAATCAACAAGTTTGTAGCAGACAAAATTGGCGTTACCCCATCGCAGGCAGCATCGTCTTCTGTCTTC</t>
+    <t>GAAGACTCTGGCGGTATCTGGAGCTCAATCAAGAATTTAGCGTCAAAAGCCTGGAATAGCGACATCGGCCAGTCACTGCGTAACAAAGCGGCGGGCGCAATCAACAAGTTTGTAGCAGACAAAATTGGCGTTACCCCATCGCAGGCAGCATCGTCGTCTGTCTTC</t>
   </si>
   <si>
     <t>id22</t>
   </si>
   <si>
-    <t>GAAGACTCTGGCGTGGGCATCGGGACGCCGATTTTCTCCTATGGCGGGGGTGCAGGGCATGTTCCCGAGTATTTCTCTTCTGTCTTC</t>
+    <t>GAAGACTCTGGCGTGGGCATCGGGACGCCGATTTTCTCCTATGGCGGGGGTGCAGGGCATGTTCCCGAGTATTTCTCGTCTGTCTTC</t>
   </si>
   <si>
     <t>id23</t>
   </si>
   <si>
-    <t>GAAGACTCTGGCCCCGACAGCGTATCCATTCCCATTACCTGTTGCTTCAATGTCATCAACCGTAAAATTCCTATCCAACGCTTGGAATCCTATACACGCATCACGAATATTCAATGCCCGAAGGAGGCTGTCATTTTCAAGACCAAACGTGGAAAAGAGGTATGTGCGGACCCGAAGGAACGCTGGGTTCGCGATTCCATGAAACATTTGGACCAAATTTTCCAGAATCTGAAGCCGTCTTCTGTCTTC</t>
+    <t>GAAGACTCTGGCCCCGACAGCGTATCCATTCCCATTACCTGTTGCTTCAATGTCATCAACCGTAAAATTCCTATCCAACGCTTGGAATCCTATACACGCATCACGAATATTCAATGCCCGAAGGAGGCTGTCATTTTCAAGACCAAACGTGGAAAAGAGGTATGTGCGGACCCGAAGGAACGCTGGGTTCGCGATTCCATGAAACATTTGGACCAAATTTTCCAGAATCTGAAGCCGTCGTCTGTCTTC</t>
   </si>
   <si>
     <t>id25</t>
   </si>
   <si>
-    <t>GAAGACTCTGGCAAGACAAAAAAGAAATTATTGAAAAAGACCTCTTCTGTCTTC</t>
+    <t>GAAGACTCTGGCAAGACAAAAAAGAAATTATTGAAAAAGACCTCGTCTGTCTTC</t>
   </si>
   <si>
     <t>id26</t>
   </si>
   <si>
-    <t>GAAGACTCTGGCTGGTATGTACGCAAATGCGCTAATAAACTGGGAACATGTCGCAAGACCTGCCGTAAGGGGGAATATCAGACAGACCCAGCCACGGGCAAGTGCTCTATCGGGAAGCTTTGTTGCATCTTGGATTTGAAGCTGGCAGGTCAATGTGGTGGAGCCGACGGCAACCAAGCGGCTGCGGGCACACAAGCAGCCGGAGGGACACGCGCTGCCGGGGGCACCCAGGGTACGGGAGGAACAGGCGCAACTGGAGCGGCAGCCACAACCGCAGCGCCCTCTTCTGTCTTC</t>
+    <t>GAAGACTCTGGCTGGTATGTACGCAAATGCGCTAATAAACTGGGAACATGTCGCAAGACCTGCCGTAAGGGGGAATATCAGACAGACCCAGCCACGGGCAAGTGCTCTATCGGGAAGCTTTGTTGCATCTTGGATTTGAAGCTGGCAGGTCAATGTGGTGGAGCCGACGGCAACCAAGCGGCTGCGGGCACACAAGCAGCCGGAGGGACACGCGCTGCCGGGGGCACCCAGGGTACGGGAGGAACAGGCGCAACTGGAGCGGCAGCCACAACCGCAGCGCCCTCGTCTGTCTTC</t>
   </si>
   <si>
     <t>id27</t>
   </si>
   <si>
-    <t>GAAGACTCTGGCGGGCGTCCTAACCCGGTGAACAATAAGCCGACCCCACATCCGCGCTTGTCTTCTGTCTTC</t>
+    <t>GAAGACTCTGGCGGGCGTCCTAACCCGGTGAACAATAAGCCGACCCCACATCCGCGCTTGTCGTCTGTCTTC</t>
   </si>
   <si>
     <t>id28</t>
   </si>
   <si>
-    <t>GAAGACTCTGGCGATTCCCATGAAGAACGTCGCCAAGGACGCCACGGACATCATGAATACGGTCGTAAGTTCCATGAGAAACATCACTCACATCGTGGGTATTCTTCTGTCTTC</t>
+    <t>GAAGACTCTGGCGATTCCCATGAAGAACGTCGCCAAGGACGCCACGGACATCATGAATACGGTCGTAAGTTCCATGAGAAACATCACTCACATCGTGGGTATTCGTCTGTCTTC</t>
   </si>
   <si>
     <t>id29</t>
   </si>
   <si>
-    <t>GAAGACTCTGGCGGTTCAAAGAAACCAGTCCCTATTATTTATTGTAATCGTCGTACGGGCAAATGTCAGCGCATGTCTTCTGTCTTC</t>
+    <t>GAAGACTCTGGCGGTTCAAAGAAACCAGTCCCTATTATTTATTGTAATCGTCGTACGGGCAAATGTCAGCGCATGTCGTCTGTCTTC</t>
   </si>
   <si>
     <t>id30</t>
   </si>
   <si>
-    <t>GAAGACTCTGGCTACAAACAATGCCACAAAAAGGGGGGACACTGCTTCCCCAAAGAAAAGATTTGTCTACCGCCCTCCTCAGATTTCGGAAAAATGGATTGTCGCTGGCGCTGGAAGTGTTGTAAGAAAGGTTCGGGGTCTTCTGTCTTC</t>
+    <t>GAAGACTCTGGCTACAAACAATGCCACAAAAAGGGGGGACACTGCTTCCCCAAAGAAAAGATTTGTCTACCGCCCTCCTCAGATTTCGGAAAAATGGATTGTCGCTGGCGCTGGAAGTGTTGTAAGAAAGGTTCGGGGTCGTCTGTCTTC</t>
   </si>
   <si>
     <t>id32</t>
   </si>
   <si>
-    <t>GAAGACTCTGGCCGCCGCTGGTGGCGCTTCTCTTCTGTCTTC</t>
+    <t>GAAGACTCTGGCCGCCGCTGGTGGCGCTTCTCGTCTGTCTTC</t>
   </si>
   <si>
     <t>id33</t>
   </si>
   <si>
-    <t>GAAGACTCTGGCACCTGTGAATCCCCCAGCCATAAGTTCAAAGGACCTTGTGCAACTAACCGTAATTGCGAATCTTCTTCTGTCTTC</t>
+    <t>GAAGACTCTGGCACCTGTGAATCCCCCAGCCATAAGTTCAAAGGACCTTGTGCAACTAACCGTAATTGCGAATCTTCGTCTGTCTTC</t>
   </si>
   <si>
     <t>id35</t>
   </si>
   <si>
-    <t>GAAGACTCTGGCTTCTTTCACCACATCTTTCGTGGAATCGTTCACGTAGGAAAGACAATCCACAAATTAGTCACGGGGTCTTCTGTCTTC</t>
+    <t>GAAGACTCTGGCTTCTTTCACCACATCTTTCGTGGAATCGTTCACGTAGGAAAGACAATCCACAAATTAGTCACGGGGTCGTCTGTCTTC</t>
   </si>
   <si>
     <t>id36</t>
   </si>
   <si>
-    <t>GAAGACTCTGGCCGCGGTGGACGCCTTTGCTACTGCCGTCGTCGTTTTTGCATTTGTGTATCTTCTGTCTTC</t>
+    <t>GAAGACTCTGGCCGCGGTGGACGCCTTTGCTACTGCCGTCGTCGTTTTTGCATTTGTGTATCGTCTGTCTTC</t>
   </si>
   <si>
     <t>id38</t>
   </si>
   <si>
-    <t>GAAGACTCTGGCGGATTACCAGTGTGTGGTGAAACCTGTTTCGGCGGGACTTGCAACACACCCGGTTGCTCTTGCACCTGGCCAATTTGTACGCGTGATTCTTCTGTCTTC</t>
+    <t>GAAGACTCTGGCGGATTACCAGTGTGTGGTGAAACCTGTTTCGGCGGGACTTGCAACACACCCGGTTGCTCTTGCACCTGGCCAATTTGTACGCGTGATTCGTCTGTCTTC</t>
   </si>
   <si>
     <t>id39</t>
   </si>
   <si>
-    <t>GAAGACTCTGGCATTCTTCCCTGGAAGTGGCCCTGGTGGCCCTGGCGTCGTTCTTCTGTCTTC</t>
+    <t>GAAGACTCTGGCATTCTTCCCTGGAAGTGGCCCTGGTGGCCCTGGCGTCGTTCGTCTGTCTTC</t>
   </si>
   <si>
     <t>id40</t>
   </si>
   <si>
-    <t>GAAGACTCTGGCGAAGAAGAATCAGAGGTCGCACACCTTCGTGTTCGTCGTGGGTTCGGTTGTCCACTTAATCAAGGAGCGTGTCACCGTCACTGCCGCTCGATTCGTCGTCGTGGAGGATACTGTTCTGGTATTATCAAGCAGACCTGCACATGCTACCGCAACTCTTCTGTCTTC</t>
+    <t>GAAGACTCTGGCGAAGAAGAATCAGAGGTCGCACACCTTCGTGTTCGTCGTGGGTTCGGTTGTCCACTTAATCAAGGAGCGTGTCACCGTCACTGCCGCTCGATTCGTCGTCGTGGAGGATACTGTTCTGGTATTATCAAGCAGACCTGCACATGCTACCGCAACTCGTCTGTCTTC</t>
   </si>
   <si>
     <t>id41</t>
   </si>
   <si>
-    <t>GAAGACTCTGGCCACGGAGTGTCGGGACACGGCCAGCACGGCGTGCACGGGTCTTCTGTCTTC</t>
+    <t>GAAGACTCTGGCCACGGAGTGTCGGGACACGGCCAGCACGGCGTGCACGGGTCGTCTGTCTTC</t>
   </si>
   <si>
     <t>rigid_linker_long</t>
   </si>
   <si>
-    <t>GAAGACAATCTTCTGCAGAGGCAGCGGCAAAGGAAGCGGCTGCAAAAGAGGCCGCAGCGAAAGAAGCAGCCGCGAAGGCTCTTGAAGCGGAAGCGGCAGCCAAAGAAGCAGCGGCTAAGGAGGCAGCCGCAAAAGAAGCAGCAGCCAAGGCGGGAATGAAGTCTTC</t>
+    <t>GAAGACAATCGTCTGCAGAGGCAGCGGCAAAGGAAGCGGCTGCAAAAGAGGCCGCAGCGAAAGAAGCAGCCGCGAAGGCTCTTGAAGCGGAAGCGGCAGCCAAAGAAGCAGCGGCTAAGGAGGCAGCCGCAAAAGAAGCAGCAGCCAAGGCGGGAATGAAGTCTTC</t>
   </si>
   <si>
     <t>rigid_linker_short</t>
   </si>
   <si>
-    <t>GAAGACAATCTTCTGGAAGCGGAATGAAGTCTTC</t>
+    <t>GAAGACAATCGTCTGGAAGCGGAATGAAGTCTTC</t>
   </si>
   <si>
     <t>flexible_linker_long</t>
   </si>
   <si>
-    <t>GAAGACAATCTTCTGGTGGGGGGGGCTCTGGCGGTGGGGGTAGTGGCGGAGGTGGTAGTGGAATGAAGTCTTC</t>
+    <t>GAAGACAATCGTCTGGTGGGGGGGGCTCTGGCGGTGGGGGTAGTGGCGGAGGTGGTAGTGGAATGAAGTCTTC</t>
   </si>
   <si>
     <t>flexible_linker_short</t>
   </si>
   <si>
-    <t>GAAGACAATCTTCTGGGGGTGGTGGCGGGGGAGGCGGAGGAATGAAGTCTTC</t>
+    <t>GAAGACAATCGTCTGGGGGTGGTGGCGGGGGAGGCGGAGGAATGAAGTCTTC</t>
   </si>
   <si>
     <t>GAAGACAAAGGTCAGCAGAGGCAGCGGCAAAGGAAGCGGCTGCAAAAGAGGCCGCAGCGAAAGAAGCAGCCGCGAAGGCTCTTGAAGCGGAAGCGGCAGCCAAAGAAGCAGCGGCTAAGGAGGCAGCCGCAAAAGAAGCAGCAGCCAAGGCGGGCGGAAAGTCTTC</t>
@@ -291,13 +291,13 @@
     <t>GAAGACGGCAGCGATGATGCCGAAGCTGTCGGCCCCGAGGCGTTCGCGGACGAAGATTTAGATGAATAATAAACTAAAGTCTTC</t>
   </si>
   <si>
+    <t>position</t>
+  </si>
+  <si>
     <t>part</t>
   </si>
   <si>
-    <t>Sequence (including restriction sites, cut sites)</t>
-  </si>
-  <si>
-    <t>position</t>
+    <t>sequence (with restriction sites, cut sites, etc.)</t>
   </si>
 </sst>
 </file>
@@ -1140,24 +1140,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="26.26953125" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C1" t="s">
         <v>92</v>
-      </c>
-      <c r="B1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C1" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -1666,6 +1661,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>